<commit_message>
Fine tuned some test data and added results_data folder
</commit_message>
<xml_diff>
--- a/knowledge-base/excel-postings/initiatives/FY 22/s1.w0/w0-workstream.initiatives.a6i.xlsx
+++ b/knowledge-base/excel-postings/initiatives/FY 22/s1.w0/w0-workstream.initiatives.a6i.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\test-knowledge-base\excel-postings\initiatives\FY 22\s1.w0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\test_db\knowledge-base\excel-postings\initiatives\FY 22\s1.w0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C102A90-4480-4661-BF14-C814DF015484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416E20BA-00DB-4E55-8C4D-C9D601B924DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{1C3C717C-D18E-4132-9B42-D7001AA1AE8F}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Analyze gaps in Finastra's ability to serve demand</t>
   </si>
   <si>
-    <t>environment</t>
-  </si>
-  <si>
     <t>Production</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>workstream.initiatives.a6i.io/v1a</t>
+  </si>
+  <si>
+    <t>knowledgeBase</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -839,10 +839,10 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -882,28 +882,28 @@
         <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>1</v>
@@ -911,71 +911,71 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="10">
         <v>44315</v>
@@ -983,10 +983,10 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1033,7 +1033,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>5</v>
@@ -1069,10 +1069,10 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="18"/>
       <c r="C4" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="14">
         <v>44377</v>
@@ -1108,7 +1108,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="14"/>
       <c r="F6" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="14">
         <v>44377</v>
@@ -1142,7 +1142,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="14"/>
       <c r="F8" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="14">
         <v>44377</v>
@@ -1165,25 +1165,25 @@
     <row r="10" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="18"/>
       <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="E10" s="14">
         <v>44484</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="14">
         <v>44439</v>
       </c>
       <c r="H10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="J10" s="13"/>
     </row>
@@ -1193,7 +1193,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="14"/>
       <c r="F11" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="14">
         <v>44439</v>
@@ -1207,7 +1207,7 @@
       <c r="D12" s="12"/>
       <c r="E12" s="14"/>
       <c r="F12" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="14">
         <v>44484</v>
@@ -1221,7 +1221,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="14"/>
       <c r="F13" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="14">
         <v>44484</v>
@@ -1233,17 +1233,17 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="14">
         <v>44530</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I14" s="12"/>
     </row>
@@ -1253,11 +1253,11 @@
       <c r="D15" s="12"/>
       <c r="E15" s="14"/>
       <c r="F15" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I15" s="12"/>
     </row>
@@ -1267,11 +1267,11 @@
       <c r="D16" s="12"/>
       <c r="E16" s="14"/>
       <c r="F16" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I16" s="12"/>
     </row>
@@ -1279,20 +1279,20 @@
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="14">
         <v>44545</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.45">
@@ -1301,7 +1301,7 @@
       <c r="D18" s="12"/>
       <c r="E18" s="14"/>
       <c r="F18" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="12"/>
@@ -1320,10 +1320,10 @@
     <row r="20" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B20" s="8"/>
       <c r="C20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="E20" s="14">
         <v>44804</v>
@@ -1347,7 +1347,7 @@
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="14">
         <v>45169</v>
@@ -1468,7 +1468,7 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B1" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -1485,34 +1485,34 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="M2" s="13"/>
     </row>
@@ -1532,16 +1532,16 @@
     <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G4" s="20">
         <v>0</v>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.45">
@@ -1576,19 +1576,19 @@
     <row r="6" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="H6" s="20">
         <v>1</v>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.45">
@@ -1701,6 +1701,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BCBD749F692D2840A5441473A3346AC8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2155aeb54e5d7003d408112aa42e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1457f3fe-6304-4719-bef8-60c608407d99" xmlns:ns3="66517581-92a9-4cb0-981f-3f6c827c3504" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4c58ad8abd1e926bea19a7235ad73cd" ns2:_="" ns3:_="">
     <xsd:import namespace="1457f3fe-6304-4719-bef8-60c608407d99"/>
@@ -1911,15 +1920,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1935,6 +1935,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F59924-779F-45B5-BAB0-46EB91D29C8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5484CF3F-DB11-4425-B875-026D7BEB7865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1953,14 +1961,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F59924-779F-45B5-BAB0-46EB91D29C8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6CD186-1AFD-40DE-A756-562BEC0234AA}">
   <ds:schemaRefs>

</xml_diff>